<commit_message>
se logro graficar los nuevos sinteticos generados
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_iris_D25_R25_Pentropia.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_iris_D25_R25_Pentropia.xlsx
@@ -659,7 +659,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.928079</t>
+          <t>2025-11-02T02:03:23.683903</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.929078</t>
+          <t>2025-11-02T02:03:23.683903</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.929078</t>
+          <t>2025-11-02T02:03:23.683903</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.929078</t>
+          <t>2025-11-02T02:03:23.684529</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.929078</t>
+          <t>2025-11-02T02:03:23.684529</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.929078</t>
+          <t>2025-11-02T02:03:23.684529</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.685075</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.685075</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.930078</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -1983,7 +1983,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -2335,7 +2335,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.686190</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2423,7 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.689327</t>
         </is>
       </c>
     </row>
@@ -2511,7 +2511,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.689753</t>
         </is>
       </c>
     </row>
@@ -2599,7 +2599,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.689753</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.690290</t>
         </is>
       </c>
     </row>
@@ -2775,7 +2775,7 @@
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.931074</t>
+          <t>2025-11-02T02:03:23.690290</t>
         </is>
       </c>
     </row>
@@ -2863,7 +2863,7 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.932074</t>
+          <t>2025-11-02T02:03:23.690290</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.932074</t>
+          <t>2025-11-02T02:03:23.690826</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-11-02T00:11:00.932074</t>
+          <t>2025-11-02T02:03:23.690826</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
agregando datasets iris y ecoli
y se agrega filtro riesgo por defecto el percentil = 50, tomando como referencia lo que aplica borderline smote
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_iris_D25_R25_Pentropia.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_iris_D25_R25_Pentropia.xlsx
@@ -659,7 +659,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.683903</t>
+          <t>2025-11-03T00:09:55.387251</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.683903</t>
+          <t>2025-11-03T00:09:55.387251</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.683903</t>
+          <t>2025-11-03T00:09:55.387251</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.684529</t>
+          <t>2025-11-03T00:09:55.387251</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.684529</t>
+          <t>2025-11-03T00:09:55.387251</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.684529</t>
+          <t>2025-11-03T00:09:55.387251</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.685075</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.685075</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -1983,7 +1983,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.388252</t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2335,7 +2335,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.686190</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2423,7 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.689327</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2511,7 +2511,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.689753</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2599,7 +2599,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.689753</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.690290</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2775,7 +2775,7 @@
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.690290</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2863,7 +2863,7 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.690290</t>
+          <t>2025-11-03T00:09:55.389252</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.690826</t>
+          <t>2025-11-03T00:09:55.390251</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-11-02T02:03:23.690826</t>
+          <t>2025-11-03T00:09:55.390251</t>
         </is>
       </c>
     </row>

</xml_diff>